<commit_message>
modify some .ipynb files
</commit_message>
<xml_diff>
--- a/raw_data/cat_deletion/deletion_fraction/YK0083/0hr/190208.xlsx
+++ b/raw_data/cat_deletion/deletion_fraction/YK0083/0hr/190208.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://univtokyo-my.sharepoint.com/personal/9898753439_utac_u-tokyo_ac_jp/Documents/FpLrT10/FpLrT10_0Hr/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuta_koganezawa/Documents/Wakamoto_lab/paper_data/Phenotypic_Buffering/raw_data/cat_deletion/deletion_fraction/YK0083/0hr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="8_{B0218412-B34F-EA47-9A28-EF2320C1F25B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EE6C91FC-1A73-914D-978D-F587BE32809E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B6D851-8D4A-384B-B1E4-8839945683B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="1020" windowWidth="25000" windowHeight="15000" activeTab="1" xr2:uid="{311E1F4D-5C11-5946-AF49-0490FFE2023F}"/>
+    <workbookView xWindow="980" yWindow="1000" windowWidth="25000" windowHeight="15000" activeTab="1" xr2:uid="{311E1F4D-5C11-5946-AF49-0490FFE2023F}"/>
   </bookViews>
   <sheets>
     <sheet name="Probability" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t xml:space="preserve">No </t>
     <phoneticPr fontId="3"/>
@@ -160,12 +163,6 @@
     <t>Pos4:0162-0238-0451:img_000000080_Txred_000</t>
   </si>
   <si>
-    <t>Pos4:0162-0241-0527:img_000000080_Txred_000</t>
-  </si>
-  <si>
-    <t>Pos4:0162-0239-0907:img_000000080_Txred_000</t>
-  </si>
-  <si>
     <t>Pos5:0162-0242-0357:img_000000080_Txred_000</t>
   </si>
   <si>
@@ -374,9 +371,6 @@
   </si>
   <si>
     <t>Pos35:0162-0600-0911:img_000000080_Txred_000</t>
-  </si>
-  <si>
-    <t>Pos35:0162-0604-0986:img_000000080_Txred_000</t>
   </si>
   <si>
     <t>Pos36:0162-0589-0382:img_000000080_Txred_000</t>
@@ -797,7 +791,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4EDD8B8-8932-B84B-AFCB-304F326004D0}">
   <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
@@ -1903,10 +1897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015B036F-A90B-964C-A99C-295994C01CAA}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:XFD86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="20"/>
@@ -1978,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K33" si="0">E2-I2</f>
+        <f t="shared" ref="K2:K31" si="0">E2-I2</f>
         <v>90.626000000000033</v>
       </c>
     </row>
@@ -2424,347 +2418,350 @@
       </c>
     </row>
     <row r="16" spans="1:11">
+      <c r="A16">
+        <v>5</v>
+      </c>
       <c r="B16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
       </c>
       <c r="D16">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="E16">
-        <v>569.43200000000002</v>
+        <v>556.00599999999997</v>
       </c>
       <c r="F16">
-        <v>42.692999999999998</v>
+        <v>39.228000000000002</v>
       </c>
       <c r="G16">
-        <v>475</v>
+        <v>456</v>
       </c>
       <c r="H16">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="I16">
-        <v>468.423</v>
+        <v>467.74</v>
       </c>
       <c r="J16">
         <v>0</v>
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>101.00900000000001</v>
+        <v>88.265999999999963</v>
       </c>
     </row>
     <row r="17" spans="1:11">
+      <c r="A17">
+        <v>7</v>
+      </c>
       <c r="B17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
       </c>
       <c r="D17">
-        <v>127</v>
+        <v>288</v>
       </c>
       <c r="E17">
-        <v>521.12599999999998</v>
+        <v>573.07600000000002</v>
       </c>
       <c r="F17">
-        <v>24.99</v>
+        <v>42.692999999999998</v>
       </c>
       <c r="G17">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="H17">
-        <v>590</v>
+        <v>671</v>
       </c>
       <c r="I17">
-        <v>464.45100000000002</v>
+        <v>469.46300000000002</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>56.674999999999955</v>
+        <v>103.613</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18">
-        <v>5</v>
-      </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
         <v>37</v>
       </c>
       <c r="D18">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="E18">
-        <v>556.00599999999997</v>
+        <v>546.23900000000003</v>
       </c>
       <c r="F18">
-        <v>39.228000000000002</v>
+        <v>36.610999999999997</v>
       </c>
       <c r="G18">
-        <v>456</v>
+        <v>472</v>
       </c>
       <c r="H18">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="I18">
-        <v>467.74</v>
+        <v>469.952</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>88.265999999999963</v>
+        <v>76.287000000000035</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19">
-        <v>7</v>
-      </c>
       <c r="B19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
       <c r="D19">
-        <v>288</v>
+        <v>156</v>
       </c>
       <c r="E19">
-        <v>573.07600000000002</v>
+        <v>495.35899999999998</v>
       </c>
       <c r="F19">
-        <v>42.692999999999998</v>
+        <v>18.077000000000002</v>
       </c>
       <c r="G19">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="H19">
-        <v>671</v>
+        <v>549</v>
       </c>
       <c r="I19">
-        <v>469.46300000000002</v>
+        <v>465.14499999999998</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>103.613</v>
+        <v>30.213999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:11">
+      <c r="A20">
+        <v>9</v>
+      </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
         <v>39</v>
       </c>
       <c r="D20">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="E20">
-        <v>546.23900000000003</v>
+        <v>605.53200000000004</v>
       </c>
       <c r="F20">
-        <v>36.610999999999997</v>
+        <v>48.16</v>
       </c>
       <c r="G20">
-        <v>472</v>
+        <v>496</v>
       </c>
       <c r="H20">
-        <v>647</v>
+        <v>709</v>
       </c>
       <c r="I20">
-        <v>469.952</v>
+        <v>473.33300000000003</v>
       </c>
       <c r="J20">
         <v>0</v>
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>76.287000000000035</v>
+        <v>132.19900000000001</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>40</v>
       </c>
       <c r="D21">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E21">
-        <v>495.35899999999998</v>
+        <v>530.59</v>
       </c>
       <c r="F21">
-        <v>18.077000000000002</v>
+        <v>31.997</v>
       </c>
       <c r="G21">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H21">
-        <v>549</v>
+        <v>606</v>
       </c>
       <c r="I21">
-        <v>465.14499999999998</v>
+        <v>467.85</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>30.213999999999999</v>
+        <v>62.740000000000009</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22">
-        <v>9</v>
-      </c>
       <c r="B22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
       </c>
       <c r="D22">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="E22">
-        <v>605.53200000000004</v>
+        <v>516.01499999999999</v>
       </c>
       <c r="F22">
-        <v>48.16</v>
+        <v>19.959</v>
       </c>
       <c r="G22">
-        <v>496</v>
+        <v>440</v>
       </c>
       <c r="H22">
-        <v>709</v>
+        <v>578</v>
       </c>
       <c r="I22">
-        <v>473.33300000000003</v>
+        <v>466.57400000000001</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>132.19900000000001</v>
+        <v>49.440999999999974</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="B23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
         <v>42</v>
       </c>
       <c r="D23">
-        <v>139</v>
+        <v>192</v>
       </c>
       <c r="E23">
-        <v>530.59</v>
+        <v>515.96900000000005</v>
       </c>
       <c r="F23">
-        <v>31.997</v>
+        <v>26.507000000000001</v>
       </c>
       <c r="G23">
-        <v>456</v>
+        <v>430</v>
       </c>
       <c r="H23">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="I23">
-        <v>467.85</v>
+        <v>465.26100000000002</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>62.740000000000009</v>
+        <v>50.708000000000027</v>
       </c>
     </row>
     <row r="24" spans="1:11">
+      <c r="A24">
+        <v>12</v>
+      </c>
       <c r="B24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
         <v>43</v>
       </c>
       <c r="D24">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="E24">
-        <v>516.01499999999999</v>
+        <v>527.024</v>
       </c>
       <c r="F24">
-        <v>19.959</v>
+        <v>25.116</v>
       </c>
       <c r="G24">
-        <v>440</v>
+        <v>469</v>
       </c>
       <c r="H24">
-        <v>578</v>
+        <v>613</v>
       </c>
       <c r="I24">
-        <v>466.57400000000001</v>
+        <v>468.56599999999997</v>
       </c>
       <c r="J24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>49.440999999999974</v>
+        <v>58.458000000000027</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="B25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
         <v>44</v>
       </c>
       <c r="D25">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="E25">
-        <v>515.96900000000005</v>
+        <v>576.27099999999996</v>
       </c>
       <c r="F25">
-        <v>26.507000000000001</v>
+        <v>37.335000000000001</v>
       </c>
       <c r="G25">
-        <v>430</v>
+        <v>492</v>
       </c>
       <c r="H25">
-        <v>596</v>
+        <v>674</v>
       </c>
       <c r="I25">
-        <v>465.26100000000002</v>
+        <v>471.02</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>50.708000000000027</v>
+        <v>105.25099999999998</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2773,29 +2770,29 @@
         <v>45</v>
       </c>
       <c r="D26">
-        <v>166</v>
+        <v>133</v>
       </c>
       <c r="E26">
-        <v>527.024</v>
+        <v>547.63199999999995</v>
       </c>
       <c r="F26">
-        <v>25.116</v>
+        <v>34.478000000000002</v>
       </c>
       <c r="G26">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="H26">
-        <v>613</v>
+        <v>622</v>
       </c>
       <c r="I26">
-        <v>468.56599999999997</v>
+        <v>468.27800000000002</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
-        <v>58.458000000000027</v>
+        <v>79.353999999999928</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -2806,34 +2803,34 @@
         <v>46</v>
       </c>
       <c r="D27">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="E27">
-        <v>576.27099999999996</v>
+        <v>526.12</v>
       </c>
       <c r="F27">
-        <v>37.335000000000001</v>
+        <v>26.486000000000001</v>
       </c>
       <c r="G27">
-        <v>492</v>
+        <v>467</v>
       </c>
       <c r="H27">
-        <v>674</v>
+        <v>587</v>
       </c>
       <c r="I27">
-        <v>471.02</v>
+        <v>462.36900000000003</v>
       </c>
       <c r="J27">
         <v>0</v>
       </c>
       <c r="K27">
         <f t="shared" si="0"/>
-        <v>105.25099999999998</v>
+        <v>63.750999999999976</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -2842,29 +2839,29 @@
         <v>47</v>
       </c>
       <c r="D28">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="E28">
-        <v>547.63199999999995</v>
+        <v>568.10299999999995</v>
       </c>
       <c r="F28">
-        <v>34.478000000000002</v>
+        <v>37.253</v>
       </c>
       <c r="G28">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="H28">
-        <v>622</v>
+        <v>635</v>
       </c>
       <c r="I28">
-        <v>468.27800000000002</v>
+        <v>471.83300000000003</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>79.353999999999928</v>
+        <v>96.269999999999925</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -2875,34 +2872,34 @@
         <v>48</v>
       </c>
       <c r="D29">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E29">
-        <v>526.12</v>
+        <v>578.846</v>
       </c>
       <c r="F29">
-        <v>26.486000000000001</v>
+        <v>45.250999999999998</v>
       </c>
       <c r="G29">
-        <v>467</v>
+        <v>484</v>
       </c>
       <c r="H29">
-        <v>587</v>
+        <v>687</v>
       </c>
       <c r="I29">
-        <v>462.36900000000003</v>
+        <v>467.63900000000001</v>
       </c>
       <c r="J29">
         <v>0</v>
       </c>
       <c r="K29">
         <f t="shared" si="0"/>
-        <v>63.750999999999976</v>
+        <v>111.20699999999999</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -2911,29 +2908,29 @@
         <v>49</v>
       </c>
       <c r="D30">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="E30">
-        <v>568.10299999999995</v>
+        <v>528.41099999999994</v>
       </c>
       <c r="F30">
-        <v>37.253</v>
+        <v>26.056999999999999</v>
       </c>
       <c r="G30">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="H30">
-        <v>635</v>
+        <v>585</v>
       </c>
       <c r="I30">
-        <v>471.83300000000003</v>
+        <v>462.80399999999997</v>
       </c>
       <c r="J30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30">
         <f t="shared" si="0"/>
-        <v>96.269999999999925</v>
+        <v>65.606999999999971</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -2944,508 +2941,508 @@
         <v>50</v>
       </c>
       <c r="D31">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="E31">
-        <v>578.846</v>
+        <v>538.63300000000004</v>
       </c>
       <c r="F31">
-        <v>45.250999999999998</v>
+        <v>27.048999999999999</v>
       </c>
       <c r="G31">
-        <v>484</v>
+        <v>469</v>
       </c>
       <c r="H31">
-        <v>687</v>
+        <v>604</v>
       </c>
       <c r="I31">
-        <v>467.63900000000001</v>
+        <v>468.15499999999997</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
-        <v>111.20699999999999</v>
+        <v>70.478000000000065</v>
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32">
-        <v>17</v>
-      </c>
       <c r="B32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
         <v>51</v>
       </c>
       <c r="D32">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="E32">
-        <v>528.41099999999994</v>
+        <v>532.92399999999998</v>
       </c>
       <c r="F32">
-        <v>26.056999999999999</v>
+        <v>31.303999999999998</v>
       </c>
       <c r="G32">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="H32">
-        <v>585</v>
+        <v>613</v>
       </c>
       <c r="I32">
-        <v>462.80399999999997</v>
+        <v>467.755</v>
       </c>
       <c r="J32">
         <v>0</v>
       </c>
       <c r="K32">
-        <f t="shared" si="0"/>
-        <v>65.606999999999971</v>
+        <f t="shared" ref="K32:K63" si="1">E32-I32</f>
+        <v>65.168999999999983</v>
       </c>
     </row>
     <row r="33" spans="1:11">
+      <c r="A33">
+        <v>18</v>
+      </c>
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
         <v>52</v>
       </c>
       <c r="D33">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E33">
-        <v>538.63300000000004</v>
+        <v>530.52599999999995</v>
       </c>
       <c r="F33">
-        <v>27.048999999999999</v>
+        <v>27.436</v>
       </c>
       <c r="G33">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="H33">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="I33">
-        <v>468.15499999999997</v>
+        <v>464.79500000000002</v>
       </c>
       <c r="J33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33">
-        <f t="shared" si="0"/>
-        <v>70.478000000000065</v>
+        <f t="shared" si="1"/>
+        <v>65.730999999999938</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="B34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
         <v>53</v>
       </c>
       <c r="D34">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="E34">
-        <v>532.92399999999998</v>
+        <v>558.42700000000002</v>
       </c>
       <c r="F34">
-        <v>31.303999999999998</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="G34">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="H34">
-        <v>613</v>
+        <v>650</v>
       </c>
       <c r="I34">
-        <v>467.755</v>
+        <v>465.71600000000001</v>
       </c>
       <c r="J34">
         <v>0</v>
       </c>
       <c r="K34">
-        <f t="shared" ref="K34:K65" si="1">E34-I34</f>
-        <v>65.168999999999983</v>
+        <f t="shared" si="1"/>
+        <v>92.711000000000013</v>
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35">
-        <v>18</v>
-      </c>
       <c r="B35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
         <v>54</v>
       </c>
       <c r="D35">
-        <v>154</v>
+        <v>177</v>
       </c>
       <c r="E35">
-        <v>530.52599999999995</v>
+        <v>525.68399999999997</v>
       </c>
       <c r="F35">
-        <v>27.436</v>
+        <v>24.72</v>
       </c>
       <c r="G35">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="H35">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="I35">
-        <v>464.79500000000002</v>
+        <v>470.01600000000002</v>
       </c>
       <c r="J35">
         <v>0</v>
       </c>
       <c r="K35">
         <f t="shared" si="1"/>
-        <v>65.730999999999938</v>
+        <v>55.66799999999995</v>
       </c>
     </row>
     <row r="36" spans="1:11">
+      <c r="A36">
+        <v>19</v>
+      </c>
       <c r="B36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" t="s">
         <v>55</v>
       </c>
       <c r="D36">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="E36">
-        <v>558.42700000000002</v>
+        <v>517.60400000000004</v>
       </c>
       <c r="F36">
-        <v>40.299999999999997</v>
+        <v>32.85</v>
       </c>
       <c r="G36">
-        <v>478</v>
+        <v>448</v>
       </c>
       <c r="H36">
-        <v>650</v>
+        <v>599</v>
       </c>
       <c r="I36">
-        <v>465.71600000000001</v>
+        <v>468.036</v>
       </c>
       <c r="J36">
         <v>0</v>
       </c>
       <c r="K36">
         <f t="shared" si="1"/>
-        <v>92.711000000000013</v>
+        <v>49.56800000000004</v>
       </c>
     </row>
     <row r="37" spans="1:11">
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
         <v>56</v>
       </c>
       <c r="D37">
-        <v>177</v>
+        <v>118</v>
       </c>
       <c r="E37">
-        <v>525.68399999999997</v>
+        <v>522.36400000000003</v>
       </c>
       <c r="F37">
-        <v>24.72</v>
+        <v>25.234000000000002</v>
       </c>
       <c r="G37">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H37">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="I37">
-        <v>470.01600000000002</v>
+        <v>464.42599999999999</v>
       </c>
       <c r="J37">
         <v>0</v>
       </c>
       <c r="K37">
         <f t="shared" si="1"/>
-        <v>55.66799999999995</v>
+        <v>57.938000000000045</v>
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38">
-        <v>19</v>
-      </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
         <v>57</v>
       </c>
       <c r="D38">
-        <v>134</v>
+        <v>187</v>
       </c>
       <c r="E38">
-        <v>517.60400000000004</v>
+        <v>551.87199999999996</v>
       </c>
       <c r="F38">
-        <v>32.85</v>
+        <v>38.493000000000002</v>
       </c>
       <c r="G38">
-        <v>448</v>
+        <v>474</v>
       </c>
       <c r="H38">
-        <v>599</v>
+        <v>636</v>
       </c>
       <c r="I38">
-        <v>468.036</v>
+        <v>466.52800000000002</v>
       </c>
       <c r="J38">
         <v>0</v>
       </c>
       <c r="K38">
         <f t="shared" si="1"/>
-        <v>49.56800000000004</v>
+        <v>85.343999999999937</v>
       </c>
     </row>
     <row r="39" spans="1:11">
       <c r="B39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
         <v>58</v>
       </c>
       <c r="D39">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E39">
-        <v>522.36400000000003</v>
+        <v>534.27</v>
       </c>
       <c r="F39">
-        <v>25.234000000000002</v>
+        <v>26.654</v>
       </c>
       <c r="G39">
-        <v>464</v>
+        <v>476</v>
       </c>
       <c r="H39">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="I39">
-        <v>464.42599999999999</v>
+        <v>466.99099999999999</v>
       </c>
       <c r="J39">
         <v>0</v>
       </c>
       <c r="K39">
         <f t="shared" si="1"/>
-        <v>57.938000000000045</v>
+        <v>67.278999999999996</v>
       </c>
     </row>
     <row r="40" spans="1:11">
       <c r="B40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
         <v>59</v>
       </c>
       <c r="D40">
-        <v>187</v>
+        <v>214</v>
       </c>
       <c r="E40">
-        <v>551.87199999999996</v>
+        <v>581.30399999999997</v>
       </c>
       <c r="F40">
-        <v>38.493000000000002</v>
+        <v>50.09</v>
       </c>
       <c r="G40">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="H40">
-        <v>636</v>
+        <v>710</v>
       </c>
       <c r="I40">
-        <v>466.52800000000002</v>
+        <v>467.76</v>
       </c>
       <c r="J40">
         <v>0</v>
       </c>
       <c r="K40">
         <f t="shared" si="1"/>
-        <v>85.343999999999937</v>
+        <v>113.54399999999998</v>
       </c>
     </row>
     <row r="41" spans="1:11">
+      <c r="A41">
+        <v>20</v>
+      </c>
       <c r="B41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s">
         <v>60</v>
       </c>
       <c r="D41">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="E41">
-        <v>534.27</v>
+        <v>538.14200000000005</v>
       </c>
       <c r="F41">
-        <v>26.654</v>
+        <v>24.577000000000002</v>
       </c>
       <c r="G41">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="H41">
-        <v>585</v>
+        <v>617</v>
       </c>
       <c r="I41">
-        <v>466.99099999999999</v>
+        <v>466.11700000000002</v>
       </c>
       <c r="J41">
         <v>0</v>
       </c>
       <c r="K41">
         <f t="shared" si="1"/>
-        <v>67.278999999999996</v>
+        <v>72.025000000000034</v>
       </c>
     </row>
     <row r="42" spans="1:11">
       <c r="B42">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
         <v>61</v>
       </c>
       <c r="D42">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="E42">
-        <v>581.30399999999997</v>
+        <v>516.11199999999997</v>
       </c>
       <c r="F42">
-        <v>50.09</v>
+        <v>26.591999999999999</v>
       </c>
       <c r="G42">
-        <v>481</v>
+        <v>449</v>
       </c>
       <c r="H42">
-        <v>710</v>
+        <v>576</v>
       </c>
       <c r="I42">
-        <v>467.76</v>
+        <v>462.48599999999999</v>
       </c>
       <c r="J42">
         <v>0</v>
       </c>
       <c r="K42">
         <f t="shared" si="1"/>
-        <v>113.54399999999998</v>
+        <v>53.625999999999976</v>
       </c>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43">
-        <v>20</v>
-      </c>
       <c r="B43">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
         <v>62</v>
       </c>
       <c r="D43">
-        <v>106</v>
+        <v>180</v>
       </c>
       <c r="E43">
-        <v>538.14200000000005</v>
+        <v>571.06100000000004</v>
       </c>
       <c r="F43">
-        <v>24.577000000000002</v>
+        <v>46.377000000000002</v>
       </c>
       <c r="G43">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="H43">
-        <v>617</v>
+        <v>670</v>
       </c>
       <c r="I43">
-        <v>466.11700000000002</v>
+        <v>467.06299999999999</v>
       </c>
       <c r="J43">
         <v>0</v>
       </c>
       <c r="K43">
         <f t="shared" si="1"/>
-        <v>72.025000000000034</v>
+        <v>103.99800000000005</v>
       </c>
     </row>
     <row r="44" spans="1:11">
+      <c r="A44">
+        <v>21</v>
+      </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>63</v>
       </c>
       <c r="D44">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="E44">
-        <v>516.11199999999997</v>
+        <v>509.98099999999999</v>
       </c>
       <c r="F44">
-        <v>26.591999999999999</v>
+        <v>22.997</v>
       </c>
       <c r="G44">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="H44">
-        <v>576</v>
+        <v>588</v>
       </c>
       <c r="I44">
-        <v>462.48599999999999</v>
+        <v>458.959</v>
       </c>
       <c r="J44">
         <v>0</v>
       </c>
       <c r="K44">
         <f t="shared" si="1"/>
-        <v>53.625999999999976</v>
+        <v>51.021999999999991</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="B45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
         <v>64</v>
       </c>
       <c r="D45">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="E45">
-        <v>571.06100000000004</v>
+        <v>514.93200000000002</v>
       </c>
       <c r="F45">
-        <v>46.377000000000002</v>
+        <v>25.681000000000001</v>
       </c>
       <c r="G45">
-        <v>479</v>
+        <v>452</v>
       </c>
       <c r="H45">
-        <v>670</v>
+        <v>574</v>
       </c>
       <c r="I45">
-        <v>467.06299999999999</v>
+        <v>462.166</v>
       </c>
       <c r="J45">
         <v>0</v>
       </c>
       <c r="K45">
         <f t="shared" si="1"/>
-        <v>103.99800000000005</v>
+        <v>52.76600000000002</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -3454,29 +3451,29 @@
         <v>65</v>
       </c>
       <c r="D46">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="E46">
-        <v>509.98099999999999</v>
+        <v>592.83000000000004</v>
       </c>
       <c r="F46">
-        <v>22.997</v>
+        <v>57.170999999999999</v>
       </c>
       <c r="G46">
-        <v>452</v>
+        <v>479</v>
       </c>
       <c r="H46">
-        <v>588</v>
+        <v>721</v>
       </c>
       <c r="I46">
-        <v>458.959</v>
+        <v>469.20100000000002</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46">
         <f t="shared" si="1"/>
-        <v>51.021999999999991</v>
+        <v>123.62900000000002</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -3487,715 +3484,715 @@
         <v>66</v>
       </c>
       <c r="D47">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E47">
-        <v>514.93200000000002</v>
+        <v>531.49599999999998</v>
       </c>
       <c r="F47">
-        <v>25.681000000000001</v>
+        <v>30.077000000000002</v>
       </c>
       <c r="G47">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="H47">
-        <v>574</v>
+        <v>602</v>
       </c>
       <c r="I47">
-        <v>462.166</v>
+        <v>464.03399999999999</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47">
         <f t="shared" si="1"/>
-        <v>52.76600000000002</v>
+        <v>67.461999999999989</v>
       </c>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48">
-        <v>22</v>
-      </c>
       <c r="B48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
         <v>67</v>
       </c>
       <c r="D48">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="E48">
-        <v>592.83000000000004</v>
+        <v>517.51</v>
       </c>
       <c r="F48">
-        <v>57.170999999999999</v>
+        <v>27.655000000000001</v>
       </c>
       <c r="G48">
-        <v>479</v>
+        <v>445</v>
       </c>
       <c r="H48">
-        <v>721</v>
+        <v>588</v>
       </c>
       <c r="I48">
-        <v>469.20100000000002</v>
+        <v>463.72199999999998</v>
       </c>
       <c r="J48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K48">
         <f t="shared" si="1"/>
-        <v>123.62900000000002</v>
+        <v>53.788000000000011</v>
       </c>
     </row>
     <row r="49" spans="1:11">
       <c r="B49">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C49" t="s">
         <v>68</v>
       </c>
       <c r="D49">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="E49">
-        <v>531.49599999999998</v>
+        <v>530.4</v>
       </c>
       <c r="F49">
-        <v>30.077000000000002</v>
+        <v>26.838000000000001</v>
       </c>
       <c r="G49">
-        <v>455</v>
+        <v>475</v>
       </c>
       <c r="H49">
         <v>602</v>
       </c>
       <c r="I49">
-        <v>464.03399999999999</v>
+        <v>460.08</v>
       </c>
       <c r="J49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49">
         <f t="shared" si="1"/>
-        <v>67.461999999999989</v>
+        <v>70.319999999999993</v>
       </c>
     </row>
     <row r="50" spans="1:11">
+      <c r="A50">
+        <v>23</v>
+      </c>
       <c r="B50">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
         <v>69</v>
       </c>
       <c r="D50">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E50">
-        <v>517.51</v>
+        <v>512.11</v>
       </c>
       <c r="F50">
-        <v>27.655000000000001</v>
+        <v>25.536999999999999</v>
       </c>
       <c r="G50">
-        <v>445</v>
+        <v>462</v>
       </c>
       <c r="H50">
-        <v>588</v>
+        <v>608</v>
       </c>
       <c r="I50">
-        <v>463.72199999999998</v>
+        <v>462.71100000000001</v>
       </c>
       <c r="J50">
         <v>0</v>
       </c>
       <c r="K50">
         <f t="shared" si="1"/>
-        <v>53.788000000000011</v>
+        <v>49.399000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:11">
       <c r="B51">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C51" t="s">
         <v>70</v>
       </c>
       <c r="D51">
-        <v>145</v>
+        <v>264</v>
       </c>
       <c r="E51">
-        <v>530.4</v>
+        <v>551.02700000000004</v>
       </c>
       <c r="F51">
-        <v>26.838000000000001</v>
+        <v>33.256999999999998</v>
       </c>
       <c r="G51">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="H51">
-        <v>602</v>
+        <v>643</v>
       </c>
       <c r="I51">
-        <v>460.08</v>
+        <v>462.39600000000002</v>
       </c>
       <c r="J51">
         <v>0</v>
       </c>
       <c r="K51">
         <f t="shared" si="1"/>
-        <v>70.319999999999993</v>
+        <v>88.631000000000029</v>
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52">
-        <v>23</v>
-      </c>
       <c r="B52">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
         <v>71</v>
       </c>
       <c r="D52">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="E52">
-        <v>512.11</v>
+        <v>580.41800000000001</v>
       </c>
       <c r="F52">
-        <v>25.536999999999999</v>
+        <v>44.234999999999999</v>
       </c>
       <c r="G52">
-        <v>462</v>
+        <v>485</v>
       </c>
       <c r="H52">
-        <v>608</v>
+        <v>661</v>
       </c>
       <c r="I52">
-        <v>462.71100000000001</v>
+        <v>462.99</v>
       </c>
       <c r="J52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52">
         <f t="shared" si="1"/>
-        <v>49.399000000000001</v>
+        <v>117.428</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="B53">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
         <v>72</v>
       </c>
       <c r="D53">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="E53">
-        <v>551.02700000000004</v>
+        <v>534.18100000000004</v>
       </c>
       <c r="F53">
-        <v>33.256999999999998</v>
+        <v>32.802999999999997</v>
       </c>
       <c r="G53">
-        <v>470</v>
+        <v>445</v>
       </c>
       <c r="H53">
-        <v>643</v>
+        <v>614</v>
       </c>
       <c r="I53">
-        <v>462.39600000000002</v>
+        <v>460.33</v>
       </c>
       <c r="J53">
         <v>0</v>
       </c>
       <c r="K53">
         <f t="shared" si="1"/>
-        <v>88.631000000000029</v>
+        <v>73.851000000000056</v>
       </c>
     </row>
     <row r="54" spans="1:11">
+      <c r="A54">
+        <v>24</v>
+      </c>
       <c r="B54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
         <v>73</v>
       </c>
       <c r="D54">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E54">
-        <v>580.41800000000001</v>
+        <v>519.26599999999996</v>
       </c>
       <c r="F54">
-        <v>44.234999999999999</v>
+        <v>27.731000000000002</v>
       </c>
       <c r="G54">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="H54">
-        <v>661</v>
+        <v>576</v>
       </c>
       <c r="I54">
-        <v>462.99</v>
+        <v>460.197</v>
       </c>
       <c r="J54">
         <v>1</v>
       </c>
       <c r="K54">
         <f t="shared" si="1"/>
-        <v>117.428</v>
+        <v>59.06899999999996</v>
       </c>
     </row>
     <row r="55" spans="1:11">
+      <c r="A55">
+        <v>25</v>
+      </c>
       <c r="B55">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C55" t="s">
         <v>74</v>
       </c>
       <c r="D55">
-        <v>249</v>
+        <v>203</v>
       </c>
       <c r="E55">
-        <v>534.18100000000004</v>
+        <v>517.92600000000004</v>
       </c>
       <c r="F55">
-        <v>32.802999999999997</v>
+        <v>26.981999999999999</v>
       </c>
       <c r="G55">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="H55">
-        <v>614</v>
+        <v>597</v>
       </c>
       <c r="I55">
-        <v>460.33</v>
+        <v>461.92599999999999</v>
       </c>
       <c r="J55">
         <v>0</v>
       </c>
       <c r="K55">
         <f t="shared" si="1"/>
-        <v>73.851000000000056</v>
+        <v>56.000000000000057</v>
       </c>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56">
-        <v>24</v>
-      </c>
       <c r="B56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
         <v>75</v>
       </c>
       <c r="D56">
-        <v>109</v>
+        <v>247</v>
       </c>
       <c r="E56">
-        <v>519.26599999999996</v>
+        <v>506.28300000000002</v>
       </c>
       <c r="F56">
-        <v>27.731000000000002</v>
+        <v>27.428999999999998</v>
       </c>
       <c r="G56">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="H56">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="I56">
-        <v>460.197</v>
+        <v>462.565</v>
       </c>
       <c r="J56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K56">
         <f t="shared" si="1"/>
-        <v>59.06899999999996</v>
+        <v>43.718000000000018</v>
       </c>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57">
-        <v>25</v>
-      </c>
       <c r="B57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C57" t="s">
         <v>76</v>
       </c>
       <c r="D57">
-        <v>203</v>
+        <v>251</v>
       </c>
       <c r="E57">
-        <v>517.92600000000004</v>
+        <v>534.45000000000005</v>
       </c>
       <c r="F57">
-        <v>26.981999999999999</v>
+        <v>38.648000000000003</v>
       </c>
       <c r="G57">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="H57">
-        <v>597</v>
+        <v>640</v>
       </c>
       <c r="I57">
-        <v>461.92599999999999</v>
+        <v>458.83199999999999</v>
       </c>
       <c r="J57">
         <v>0</v>
       </c>
       <c r="K57">
         <f t="shared" si="1"/>
-        <v>56.000000000000057</v>
+        <v>75.618000000000052</v>
       </c>
     </row>
     <row r="58" spans="1:11">
+      <c r="A58">
+        <v>26</v>
+      </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
         <v>77</v>
       </c>
       <c r="D58">
-        <v>247</v>
+        <v>364</v>
       </c>
       <c r="E58">
-        <v>506.28300000000002</v>
+        <v>520.94500000000005</v>
       </c>
       <c r="F58">
-        <v>27.428999999999998</v>
+        <v>35.881</v>
       </c>
       <c r="G58">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H58">
-        <v>578</v>
+        <v>620</v>
       </c>
       <c r="I58">
-        <v>462.565</v>
+        <v>460.55799999999999</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K58">
         <f t="shared" si="1"/>
-        <v>43.718000000000018</v>
+        <v>60.387000000000057</v>
       </c>
     </row>
     <row r="59" spans="1:11">
       <c r="B59">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
         <v>78</v>
       </c>
       <c r="D59">
-        <v>251</v>
+        <v>137</v>
       </c>
       <c r="E59">
-        <v>534.45000000000005</v>
+        <v>544.78800000000001</v>
       </c>
       <c r="F59">
-        <v>38.648000000000003</v>
+        <v>45.710999999999999</v>
       </c>
       <c r="G59">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="H59">
-        <v>640</v>
+        <v>649</v>
       </c>
       <c r="I59">
-        <v>458.83199999999999</v>
+        <v>465.18200000000002</v>
       </c>
       <c r="J59">
         <v>0</v>
       </c>
       <c r="K59">
         <f t="shared" si="1"/>
-        <v>75.618000000000052</v>
+        <v>79.605999999999995</v>
       </c>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60">
-        <v>26</v>
-      </c>
       <c r="B60">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
         <v>79</v>
       </c>
       <c r="D60">
-        <v>364</v>
+        <v>134</v>
       </c>
       <c r="E60">
-        <v>520.94500000000005</v>
+        <v>569.28399999999999</v>
       </c>
       <c r="F60">
-        <v>35.881</v>
+        <v>40.762999999999998</v>
       </c>
       <c r="G60">
-        <v>446</v>
+        <v>476</v>
       </c>
       <c r="H60">
-        <v>620</v>
+        <v>658</v>
       </c>
       <c r="I60">
-        <v>460.55799999999999</v>
+        <v>463.65699999999998</v>
       </c>
       <c r="J60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60">
         <f t="shared" si="1"/>
-        <v>60.387000000000057</v>
+        <v>105.62700000000001</v>
       </c>
     </row>
     <row r="61" spans="1:11">
       <c r="B61">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C61" t="s">
         <v>80</v>
       </c>
       <c r="D61">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="E61">
-        <v>544.78800000000001</v>
+        <v>600.48699999999997</v>
       </c>
       <c r="F61">
-        <v>45.710999999999999</v>
+        <v>60.573999999999998</v>
       </c>
       <c r="G61">
-        <v>451</v>
+        <v>480</v>
       </c>
       <c r="H61">
-        <v>649</v>
+        <v>732</v>
       </c>
       <c r="I61">
-        <v>465.18200000000002</v>
+        <v>463.096</v>
       </c>
       <c r="J61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K61">
         <f t="shared" si="1"/>
-        <v>79.605999999999995</v>
+        <v>137.39099999999996</v>
       </c>
     </row>
     <row r="62" spans="1:11">
+      <c r="A62">
+        <v>27</v>
+      </c>
       <c r="B62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C62" t="s">
         <v>81</v>
       </c>
       <c r="D62">
-        <v>134</v>
+        <v>229</v>
       </c>
       <c r="E62">
-        <v>569.28399999999999</v>
+        <v>537.07899999999995</v>
       </c>
       <c r="F62">
-        <v>40.762999999999998</v>
+        <v>30.760999999999999</v>
       </c>
       <c r="G62">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="H62">
-        <v>658</v>
+        <v>613</v>
       </c>
       <c r="I62">
-        <v>463.65699999999998</v>
+        <v>466.55099999999999</v>
       </c>
       <c r="J62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K62">
         <f t="shared" si="1"/>
-        <v>105.62700000000001</v>
+        <v>70.527999999999963</v>
       </c>
     </row>
     <row r="63" spans="1:11">
       <c r="B63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
         <v>82</v>
       </c>
       <c r="D63">
-        <v>158</v>
+        <v>109</v>
       </c>
       <c r="E63">
-        <v>600.48699999999997</v>
+        <v>544.99099999999999</v>
       </c>
       <c r="F63">
-        <v>60.573999999999998</v>
+        <v>30.904</v>
       </c>
       <c r="G63">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="H63">
-        <v>732</v>
+        <v>620</v>
       </c>
       <c r="I63">
-        <v>463.096</v>
+        <v>465.86900000000003</v>
       </c>
       <c r="J63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K63">
         <f t="shared" si="1"/>
-        <v>137.39099999999996</v>
+        <v>79.121999999999957</v>
       </c>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64">
-        <v>27</v>
-      </c>
       <c r="B64">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
         <v>83</v>
       </c>
       <c r="D64">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="E64">
-        <v>537.07899999999995</v>
+        <v>523.18799999999999</v>
       </c>
       <c r="F64">
-        <v>30.760999999999999</v>
+        <v>24.901</v>
       </c>
       <c r="G64">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="H64">
-        <v>613</v>
+        <v>578</v>
       </c>
       <c r="I64">
-        <v>466.55099999999999</v>
+        <v>465.22</v>
       </c>
       <c r="J64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K64">
-        <f t="shared" si="1"/>
-        <v>70.527999999999963</v>
+        <f t="shared" ref="K64:K98" si="2">E64-I64</f>
+        <v>57.967999999999961</v>
       </c>
     </row>
     <row r="65" spans="1:11">
+      <c r="A65">
+        <v>28</v>
+      </c>
       <c r="B65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
         <v>84</v>
       </c>
       <c r="D65">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="E65">
-        <v>544.99099999999999</v>
+        <v>567.22299999999996</v>
       </c>
       <c r="F65">
-        <v>30.904</v>
+        <v>39.744</v>
       </c>
       <c r="G65">
-        <v>481</v>
+        <v>469</v>
       </c>
       <c r="H65">
-        <v>620</v>
+        <v>668</v>
       </c>
       <c r="I65">
-        <v>465.86900000000003</v>
+        <v>467.23200000000003</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K65">
-        <f t="shared" si="1"/>
-        <v>79.121999999999957</v>
+        <f t="shared" si="2"/>
+        <v>99.990999999999929</v>
       </c>
     </row>
     <row r="66" spans="1:11">
+      <c r="A66">
+        <v>30</v>
+      </c>
       <c r="B66">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
         <v>85</v>
       </c>
       <c r="D66">
-        <v>234</v>
+        <v>185</v>
       </c>
       <c r="E66">
-        <v>523.18799999999999</v>
+        <v>522.21100000000001</v>
       </c>
       <c r="F66">
-        <v>24.901</v>
+        <v>28.297999999999998</v>
       </c>
       <c r="G66">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H66">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="I66">
-        <v>465.22</v>
+        <v>460.97199999999998</v>
       </c>
       <c r="J66">
         <v>0</v>
       </c>
       <c r="K66">
-        <f t="shared" ref="K66:K101" si="2">E66-I66</f>
-        <v>57.967999999999961</v>
+        <f t="shared" si="2"/>
+        <v>61.239000000000033</v>
       </c>
     </row>
     <row r="67" spans="1:11">
-      <c r="A67">
-        <v>28</v>
-      </c>
       <c r="B67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C67" t="s">
         <v>86</v>
       </c>
       <c r="D67">
-        <v>130</v>
+        <v>303</v>
       </c>
       <c r="E67">
-        <v>567.22299999999996</v>
+        <v>543.58699999999999</v>
       </c>
       <c r="F67">
-        <v>39.744</v>
+        <v>34.165999999999997</v>
       </c>
       <c r="G67">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="H67">
-        <v>668</v>
+        <v>619</v>
       </c>
       <c r="I67">
-        <v>467.23200000000003</v>
+        <v>466.51</v>
       </c>
       <c r="J67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K67">
         <f t="shared" si="2"/>
-        <v>99.990999999999929</v>
+        <v>77.076999999999998</v>
       </c>
     </row>
     <row r="68" spans="1:11">
       <c r="A68">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -4204,29 +4201,29 @@
         <v>87</v>
       </c>
       <c r="D68">
-        <v>185</v>
+        <v>80</v>
       </c>
       <c r="E68">
-        <v>522.21100000000001</v>
+        <v>513.5</v>
       </c>
       <c r="F68">
-        <v>28.297999999999998</v>
+        <v>18.369</v>
       </c>
       <c r="G68">
-        <v>457</v>
+        <v>472</v>
       </c>
       <c r="H68">
-        <v>581</v>
+        <v>556</v>
       </c>
       <c r="I68">
-        <v>460.97199999999998</v>
+        <v>463.767</v>
       </c>
       <c r="J68">
         <v>0</v>
       </c>
       <c r="K68">
         <f t="shared" si="2"/>
-        <v>61.239000000000033</v>
+        <v>49.733000000000004</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -4237,34 +4234,34 @@
         <v>88</v>
       </c>
       <c r="D69">
-        <v>303</v>
+        <v>139</v>
       </c>
       <c r="E69">
-        <v>543.58699999999999</v>
+        <v>559.33799999999997</v>
       </c>
       <c r="F69">
-        <v>34.165999999999997</v>
+        <v>39.996000000000002</v>
       </c>
       <c r="G69">
-        <v>455</v>
+        <v>480</v>
       </c>
       <c r="H69">
-        <v>619</v>
+        <v>657</v>
       </c>
       <c r="I69">
-        <v>466.51</v>
+        <v>463.15199999999999</v>
       </c>
       <c r="J69">
         <v>0</v>
       </c>
       <c r="K69">
         <f t="shared" si="2"/>
-        <v>77.076999999999998</v>
+        <v>96.185999999999979</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -4273,29 +4270,29 @@
         <v>89</v>
       </c>
       <c r="D70">
-        <v>80</v>
+        <v>121</v>
       </c>
       <c r="E70">
-        <v>513.5</v>
+        <v>527.04100000000005</v>
       </c>
       <c r="F70">
-        <v>18.369</v>
+        <v>32.47</v>
       </c>
       <c r="G70">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="H70">
-        <v>556</v>
+        <v>607</v>
       </c>
       <c r="I70">
-        <v>463.767</v>
+        <v>459.89499999999998</v>
       </c>
       <c r="J70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K70">
         <f t="shared" si="2"/>
-        <v>49.733000000000004</v>
+        <v>67.146000000000072</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -4306,1045 +4303,943 @@
         <v>90</v>
       </c>
       <c r="D71">
-        <v>139</v>
+        <v>191</v>
       </c>
       <c r="E71">
-        <v>559.33799999999997</v>
+        <v>536.43499999999995</v>
       </c>
       <c r="F71">
-        <v>39.996000000000002</v>
+        <v>33.529000000000003</v>
       </c>
       <c r="G71">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="H71">
-        <v>657</v>
+        <v>617</v>
       </c>
       <c r="I71">
-        <v>463.15199999999999</v>
+        <v>464.19099999999997</v>
       </c>
       <c r="J71">
         <v>0</v>
       </c>
       <c r="K71">
         <f t="shared" si="2"/>
-        <v>96.185999999999979</v>
+        <v>72.243999999999971</v>
       </c>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72">
-        <v>32</v>
-      </c>
       <c r="B72">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C72" t="s">
         <v>91</v>
       </c>
       <c r="D72">
-        <v>121</v>
+        <v>204</v>
       </c>
       <c r="E72">
-        <v>527.04100000000005</v>
+        <v>530.57399999999996</v>
       </c>
       <c r="F72">
-        <v>32.47</v>
+        <v>29.882999999999999</v>
       </c>
       <c r="G72">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="H72">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="I72">
-        <v>459.89499999999998</v>
+        <v>461.65</v>
       </c>
       <c r="J72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K72">
         <f t="shared" si="2"/>
-        <v>67.146000000000072</v>
+        <v>68.923999999999978</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="B73">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C73" t="s">
         <v>92</v>
       </c>
       <c r="D73">
-        <v>191</v>
+        <v>291</v>
       </c>
       <c r="E73">
-        <v>536.43499999999995</v>
+        <v>511.065</v>
       </c>
       <c r="F73">
-        <v>33.529000000000003</v>
+        <v>25.623000000000001</v>
       </c>
       <c r="G73">
-        <v>463</v>
+        <v>437</v>
       </c>
       <c r="H73">
-        <v>617</v>
+        <v>589</v>
       </c>
       <c r="I73">
-        <v>464.19099999999997</v>
+        <v>463.56</v>
       </c>
       <c r="J73">
         <v>0</v>
       </c>
       <c r="K73">
         <f t="shared" si="2"/>
-        <v>72.243999999999971</v>
+        <v>47.504999999999995</v>
       </c>
     </row>
     <row r="74" spans="1:11">
       <c r="B74">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C74" t="s">
         <v>93</v>
       </c>
       <c r="D74">
-        <v>204</v>
+        <v>235</v>
       </c>
       <c r="E74">
-        <v>530.57399999999996</v>
+        <v>530.43399999999997</v>
       </c>
       <c r="F74">
-        <v>29.882999999999999</v>
+        <v>32.033999999999999</v>
       </c>
       <c r="G74">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="H74">
-        <v>610</v>
+        <v>619</v>
       </c>
       <c r="I74">
-        <v>461.65</v>
+        <v>464.07</v>
       </c>
       <c r="J74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K74">
         <f t="shared" si="2"/>
-        <v>68.923999999999978</v>
+        <v>66.363999999999976</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="B75">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s">
         <v>94</v>
       </c>
       <c r="D75">
-        <v>291</v>
+        <v>172</v>
       </c>
       <c r="E75">
-        <v>511.065</v>
+        <v>551.85500000000002</v>
       </c>
       <c r="F75">
-        <v>25.623000000000001</v>
+        <v>41.335999999999999</v>
       </c>
       <c r="G75">
-        <v>437</v>
+        <v>474</v>
       </c>
       <c r="H75">
-        <v>589</v>
+        <v>671</v>
       </c>
       <c r="I75">
-        <v>463.56</v>
+        <v>463.75</v>
       </c>
       <c r="J75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K75">
         <f t="shared" si="2"/>
-        <v>47.504999999999995</v>
+        <v>88.105000000000018</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="B76">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C76" t="s">
         <v>95</v>
       </c>
       <c r="D76">
-        <v>235</v>
+        <v>177</v>
       </c>
       <c r="E76">
-        <v>530.43399999999997</v>
+        <v>534.81399999999996</v>
       </c>
       <c r="F76">
-        <v>32.033999999999999</v>
+        <v>34.874000000000002</v>
       </c>
       <c r="G76">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="H76">
-        <v>619</v>
+        <v>628</v>
       </c>
       <c r="I76">
-        <v>464.07</v>
+        <v>463.96199999999999</v>
       </c>
       <c r="J76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K76">
         <f t="shared" si="2"/>
-        <v>66.363999999999976</v>
+        <v>70.851999999999975</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="B77">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C77" t="s">
         <v>96</v>
       </c>
       <c r="D77">
-        <v>172</v>
+        <v>103</v>
       </c>
       <c r="E77">
-        <v>551.85500000000002</v>
+        <v>513.88300000000004</v>
       </c>
       <c r="F77">
-        <v>41.335999999999999</v>
+        <v>25.06</v>
       </c>
       <c r="G77">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="H77">
-        <v>671</v>
+        <v>581</v>
       </c>
       <c r="I77">
-        <v>463.75</v>
+        <v>461.47399999999999</v>
       </c>
       <c r="J77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K77">
         <f t="shared" si="2"/>
-        <v>88.105000000000018</v>
+        <v>52.409000000000049</v>
       </c>
     </row>
     <row r="78" spans="1:11">
+      <c r="A78">
+        <v>33</v>
+      </c>
       <c r="B78">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C78" t="s">
         <v>97</v>
       </c>
       <c r="D78">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="E78">
-        <v>534.81399999999996</v>
+        <v>530.49199999999996</v>
       </c>
       <c r="F78">
-        <v>34.874000000000002</v>
+        <v>34.103999999999999</v>
       </c>
       <c r="G78">
-        <v>474</v>
+        <v>454</v>
       </c>
       <c r="H78">
-        <v>628</v>
+        <v>618</v>
       </c>
       <c r="I78">
-        <v>463.96199999999999</v>
+        <v>463.16800000000001</v>
       </c>
       <c r="J78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K78">
         <f t="shared" si="2"/>
-        <v>70.851999999999975</v>
+        <v>67.323999999999955</v>
       </c>
     </row>
     <row r="79" spans="1:11">
       <c r="B79">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C79" t="s">
         <v>98</v>
       </c>
       <c r="D79">
-        <v>103</v>
+        <v>329</v>
       </c>
       <c r="E79">
-        <v>513.88300000000004</v>
+        <v>524.67200000000003</v>
       </c>
       <c r="F79">
-        <v>25.06</v>
+        <v>29.010999999999999</v>
       </c>
       <c r="G79">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H79">
-        <v>581</v>
+        <v>629</v>
       </c>
       <c r="I79">
-        <v>461.47399999999999</v>
+        <v>464.56099999999998</v>
       </c>
       <c r="J79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K79">
         <f t="shared" si="2"/>
-        <v>52.409000000000049</v>
+        <v>60.111000000000047</v>
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80">
-        <v>33</v>
-      </c>
       <c r="B80">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C80" t="s">
         <v>99</v>
       </c>
       <c r="D80">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E80">
-        <v>530.49199999999996</v>
+        <v>520.22900000000004</v>
       </c>
       <c r="F80">
-        <v>34.103999999999999</v>
+        <v>25.911000000000001</v>
       </c>
       <c r="G80">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="H80">
-        <v>618</v>
+        <v>588</v>
       </c>
       <c r="I80">
-        <v>463.16800000000001</v>
+        <v>462.125</v>
       </c>
       <c r="J80">
         <v>1</v>
       </c>
       <c r="K80">
         <f t="shared" si="2"/>
-        <v>67.323999999999955</v>
+        <v>58.104000000000042</v>
       </c>
     </row>
     <row r="81" spans="1:11">
+      <c r="A81">
+        <v>34</v>
+      </c>
       <c r="B81">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C81" t="s">
         <v>100</v>
       </c>
       <c r="D81">
-        <v>329</v>
+        <v>198</v>
       </c>
       <c r="E81">
-        <v>524.67200000000003</v>
+        <v>498.14100000000002</v>
       </c>
       <c r="F81">
-        <v>29.010999999999999</v>
+        <v>19.202000000000002</v>
       </c>
       <c r="G81">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="H81">
-        <v>629</v>
+        <v>547</v>
       </c>
       <c r="I81">
-        <v>464.56099999999998</v>
+        <v>460.04300000000001</v>
       </c>
       <c r="J81">
         <v>1</v>
       </c>
       <c r="K81">
         <f t="shared" si="2"/>
-        <v>60.111000000000047</v>
+        <v>38.098000000000013</v>
       </c>
     </row>
     <row r="82" spans="1:11">
+      <c r="A82">
+        <v>35</v>
+      </c>
       <c r="B82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C82" t="s">
         <v>101</v>
       </c>
       <c r="D82">
-        <v>109</v>
+        <v>195</v>
       </c>
       <c r="E82">
-        <v>520.22900000000004</v>
+        <v>544.32299999999998</v>
       </c>
       <c r="F82">
-        <v>25.911000000000001</v>
+        <v>32.948999999999998</v>
       </c>
       <c r="G82">
-        <v>460</v>
+        <v>476</v>
       </c>
       <c r="H82">
-        <v>588</v>
+        <v>632</v>
       </c>
       <c r="I82">
-        <v>462.125</v>
+        <v>464.34100000000001</v>
       </c>
       <c r="J82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K82">
         <f t="shared" si="2"/>
-        <v>58.104000000000042</v>
+        <v>79.981999999999971</v>
       </c>
     </row>
     <row r="83" spans="1:11">
-      <c r="A83">
-        <v>34</v>
-      </c>
       <c r="B83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C83" t="s">
         <v>102</v>
       </c>
       <c r="D83">
-        <v>198</v>
+        <v>446</v>
       </c>
       <c r="E83">
-        <v>498.14100000000002</v>
+        <v>528.303</v>
       </c>
       <c r="F83">
-        <v>19.202000000000002</v>
+        <v>26.135999999999999</v>
       </c>
       <c r="G83">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="H83">
-        <v>547</v>
+        <v>613</v>
       </c>
       <c r="I83">
-        <v>460.04300000000001</v>
+        <v>465.01499999999999</v>
       </c>
       <c r="J83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K83">
         <f t="shared" si="2"/>
-        <v>38.098000000000013</v>
+        <v>63.288000000000011</v>
       </c>
     </row>
     <row r="84" spans="1:11">
-      <c r="A84">
-        <v>35</v>
-      </c>
       <c r="B84">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C84" t="s">
         <v>103</v>
       </c>
       <c r="D84">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="E84">
-        <v>544.32299999999998</v>
+        <v>492.11799999999999</v>
       </c>
       <c r="F84">
-        <v>32.948999999999998</v>
+        <v>17.922000000000001</v>
       </c>
       <c r="G84">
-        <v>476</v>
+        <v>446</v>
       </c>
       <c r="H84">
-        <v>632</v>
+        <v>531</v>
       </c>
       <c r="I84">
-        <v>464.34100000000001</v>
+        <v>462.16</v>
       </c>
       <c r="J84">
         <v>0</v>
       </c>
       <c r="K84">
         <f t="shared" si="2"/>
-        <v>79.981999999999971</v>
+        <v>29.95799999999997</v>
       </c>
     </row>
     <row r="85" spans="1:11">
       <c r="B85">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C85" t="s">
         <v>104</v>
       </c>
       <c r="D85">
-        <v>446</v>
+        <v>244</v>
       </c>
       <c r="E85">
-        <v>528.303</v>
+        <v>500.197</v>
       </c>
       <c r="F85">
-        <v>26.135999999999999</v>
+        <v>18.927</v>
       </c>
       <c r="G85">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="H85">
-        <v>613</v>
+        <v>552</v>
       </c>
       <c r="I85">
-        <v>465.01499999999999</v>
+        <v>459.47300000000001</v>
       </c>
       <c r="J85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K85">
         <f t="shared" si="2"/>
-        <v>63.288000000000011</v>
+        <v>40.72399999999999</v>
       </c>
     </row>
     <row r="86" spans="1:11">
+      <c r="A86">
+        <v>36</v>
+      </c>
       <c r="B86">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86" t="s">
         <v>105</v>
       </c>
       <c r="D86">
-        <v>169</v>
+        <v>99</v>
       </c>
       <c r="E86">
-        <v>492.11799999999999</v>
+        <v>543.53499999999997</v>
       </c>
       <c r="F86">
-        <v>17.922000000000001</v>
+        <v>31.638999999999999</v>
       </c>
       <c r="G86">
-        <v>446</v>
+        <v>480</v>
       </c>
       <c r="H86">
-        <v>531</v>
+        <v>619</v>
       </c>
       <c r="I86">
-        <v>462.16</v>
+        <v>463.88200000000001</v>
       </c>
       <c r="J86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K86">
         <f t="shared" si="2"/>
-        <v>29.95799999999997</v>
+        <v>79.652999999999963</v>
       </c>
     </row>
     <row r="87" spans="1:11">
       <c r="B87">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C87" t="s">
         <v>106</v>
       </c>
       <c r="D87">
-        <v>244</v>
+        <v>150</v>
       </c>
       <c r="E87">
-        <v>500.197</v>
+        <v>563.08000000000004</v>
       </c>
       <c r="F87">
-        <v>18.927</v>
+        <v>36.585999999999999</v>
       </c>
       <c r="G87">
-        <v>448</v>
+        <v>484</v>
       </c>
       <c r="H87">
-        <v>552</v>
+        <v>662</v>
       </c>
       <c r="I87">
-        <v>459.47300000000001</v>
+        <v>463.036</v>
       </c>
       <c r="J87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K87">
         <f t="shared" si="2"/>
-        <v>40.72399999999999</v>
+        <v>100.04400000000004</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="B88">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C88" t="s">
         <v>107</v>
       </c>
       <c r="D88">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="E88">
-        <v>485.95800000000003</v>
+        <v>509.767</v>
       </c>
       <c r="F88">
-        <v>15.134</v>
+        <v>23.373000000000001</v>
       </c>
       <c r="G88">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="H88">
-        <v>540</v>
+        <v>568</v>
       </c>
       <c r="I88">
-        <v>460.46300000000002</v>
+        <v>462.81099999999998</v>
       </c>
       <c r="J88">
         <v>0</v>
       </c>
       <c r="K88">
         <f t="shared" si="2"/>
-        <v>25.495000000000005</v>
+        <v>46.956000000000017</v>
       </c>
     </row>
     <row r="89" spans="1:11">
-      <c r="A89">
-        <v>36</v>
-      </c>
       <c r="B89">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C89" t="s">
         <v>108</v>
       </c>
       <c r="D89">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="E89">
-        <v>543.53499999999997</v>
+        <v>542.63699999999994</v>
       </c>
       <c r="F89">
-        <v>31.638999999999999</v>
+        <v>39.368000000000002</v>
       </c>
       <c r="G89">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="H89">
-        <v>619</v>
+        <v>632</v>
       </c>
       <c r="I89">
-        <v>463.88200000000001</v>
+        <v>464.42200000000003</v>
       </c>
       <c r="J89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K89">
         <f t="shared" si="2"/>
-        <v>79.652999999999963</v>
+        <v>78.214999999999918</v>
       </c>
     </row>
     <row r="90" spans="1:11">
       <c r="B90">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C90" t="s">
         <v>109</v>
       </c>
       <c r="D90">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="E90">
-        <v>563.08000000000004</v>
+        <v>507.61500000000001</v>
       </c>
       <c r="F90">
-        <v>36.585999999999999</v>
+        <v>21.788</v>
       </c>
       <c r="G90">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="H90">
-        <v>662</v>
+        <v>564</v>
       </c>
       <c r="I90">
-        <v>463.036</v>
+        <v>462.30700000000002</v>
       </c>
       <c r="J90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K90">
         <f t="shared" si="2"/>
-        <v>100.04400000000004</v>
+        <v>45.307999999999993</v>
       </c>
     </row>
     <row r="91" spans="1:11">
+      <c r="A91">
+        <v>37</v>
+      </c>
       <c r="B91">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C91" t="s">
         <v>110</v>
       </c>
       <c r="D91">
-        <v>219</v>
+        <v>138</v>
       </c>
       <c r="E91">
-        <v>509.767</v>
+        <v>524.529</v>
       </c>
       <c r="F91">
-        <v>23.373000000000001</v>
+        <v>28.606000000000002</v>
       </c>
       <c r="G91">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="H91">
-        <v>568</v>
+        <v>612</v>
       </c>
       <c r="I91">
-        <v>462.81099999999998</v>
+        <v>463.57299999999998</v>
       </c>
       <c r="J91">
         <v>0</v>
       </c>
       <c r="K91">
         <f t="shared" si="2"/>
-        <v>46.956000000000017</v>
+        <v>60.956000000000017</v>
       </c>
     </row>
     <row r="92" spans="1:11">
       <c r="B92">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C92" t="s">
         <v>111</v>
       </c>
       <c r="D92">
-        <v>157</v>
+        <v>203</v>
       </c>
       <c r="E92">
-        <v>542.63699999999994</v>
+        <v>501.46800000000002</v>
       </c>
       <c r="F92">
-        <v>39.368000000000002</v>
+        <v>23.077000000000002</v>
       </c>
       <c r="G92">
-        <v>479</v>
+        <v>421</v>
       </c>
       <c r="H92">
-        <v>632</v>
+        <v>573</v>
       </c>
       <c r="I92">
-        <v>464.42200000000003</v>
+        <v>462.53</v>
       </c>
       <c r="J92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K92">
         <f t="shared" si="2"/>
-        <v>78.214999999999918</v>
+        <v>38.938000000000045</v>
       </c>
     </row>
     <row r="93" spans="1:11">
       <c r="B93">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C93" t="s">
         <v>112</v>
       </c>
       <c r="D93">
-        <v>130</v>
+        <v>222</v>
       </c>
       <c r="E93">
-        <v>507.61500000000001</v>
+        <v>510.923</v>
       </c>
       <c r="F93">
-        <v>21.788</v>
+        <v>19.495999999999999</v>
       </c>
       <c r="G93">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="H93">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="I93">
-        <v>462.30700000000002</v>
+        <v>464.50299999999999</v>
       </c>
       <c r="J93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K93">
         <f t="shared" si="2"/>
-        <v>45.307999999999993</v>
+        <v>46.420000000000016</v>
       </c>
     </row>
     <row r="94" spans="1:11">
-      <c r="A94">
-        <v>37</v>
-      </c>
       <c r="B94">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C94" t="s">
         <v>113</v>
       </c>
       <c r="D94">
-        <v>138</v>
+        <v>246</v>
       </c>
       <c r="E94">
-        <v>524.529</v>
+        <v>500.01600000000002</v>
       </c>
       <c r="F94">
-        <v>28.606000000000002</v>
+        <v>18.87</v>
       </c>
       <c r="G94">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="H94">
-        <v>612</v>
+        <v>561</v>
       </c>
       <c r="I94">
-        <v>463.57299999999998</v>
+        <v>465.86500000000001</v>
       </c>
       <c r="J94">
         <v>0</v>
       </c>
       <c r="K94">
         <f t="shared" si="2"/>
-        <v>60.956000000000017</v>
+        <v>34.15100000000001</v>
       </c>
     </row>
     <row r="95" spans="1:11">
       <c r="B95">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C95" t="s">
         <v>114</v>
       </c>
       <c r="D95">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="E95">
-        <v>501.46800000000002</v>
+        <v>498.25900000000001</v>
       </c>
       <c r="F95">
-        <v>23.077000000000002</v>
+        <v>18.375</v>
       </c>
       <c r="G95">
-        <v>421</v>
+        <v>456</v>
       </c>
       <c r="H95">
-        <v>573</v>
+        <v>556</v>
       </c>
       <c r="I95">
-        <v>462.53</v>
+        <v>459.83</v>
       </c>
       <c r="J95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K95">
         <f t="shared" si="2"/>
-        <v>38.938000000000045</v>
+        <v>38.42900000000003</v>
       </c>
     </row>
     <row r="96" spans="1:11">
+      <c r="A96">
+        <v>38</v>
+      </c>
       <c r="B96">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C96" t="s">
         <v>115</v>
       </c>
       <c r="D96">
-        <v>222</v>
+        <v>96</v>
       </c>
       <c r="E96">
-        <v>510.923</v>
+        <v>604.85400000000004</v>
       </c>
       <c r="F96">
-        <v>19.495999999999999</v>
+        <v>47.061999999999998</v>
       </c>
       <c r="G96">
-        <v>454</v>
+        <v>508</v>
       </c>
       <c r="H96">
-        <v>565</v>
+        <v>691</v>
       </c>
       <c r="I96">
-        <v>464.50299999999999</v>
+        <v>465.54500000000002</v>
       </c>
       <c r="J96">
         <v>0</v>
       </c>
       <c r="K96">
         <f t="shared" si="2"/>
-        <v>46.420000000000016</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11">
+        <v>139.30900000000003</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11">
       <c r="B97">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C97" t="s">
         <v>116</v>
       </c>
       <c r="D97">
-        <v>246</v>
+        <v>173</v>
       </c>
       <c r="E97">
-        <v>500.01600000000002</v>
+        <v>500.08699999999999</v>
       </c>
       <c r="F97">
-        <v>18.87</v>
+        <v>21.128</v>
       </c>
       <c r="G97">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="H97">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="I97">
-        <v>465.86500000000001</v>
+        <v>461.05399999999997</v>
       </c>
       <c r="J97">
         <v>0</v>
       </c>
       <c r="K97">
         <f t="shared" si="2"/>
-        <v>34.15100000000001</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11">
+        <v>39.033000000000015</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11">
       <c r="B98">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C98" t="s">
         <v>117</v>
       </c>
       <c r="D98">
-        <v>224</v>
+        <v>123</v>
       </c>
       <c r="E98">
-        <v>498.25900000000001</v>
+        <v>485.512</v>
       </c>
       <c r="F98">
-        <v>18.375</v>
+        <v>16.664000000000001</v>
       </c>
       <c r="G98">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="H98">
-        <v>556</v>
+        <v>532</v>
       </c>
       <c r="I98">
-        <v>459.83</v>
+        <v>459.43200000000002</v>
       </c>
       <c r="J98">
         <v>0</v>
       </c>
       <c r="K98">
         <f t="shared" si="2"/>
-        <v>38.42900000000003</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11">
-      <c r="A99">
-        <v>38</v>
-      </c>
-      <c r="B99">
-        <v>1</v>
-      </c>
-      <c r="C99" t="s">
-        <v>118</v>
-      </c>
-      <c r="D99">
-        <v>96</v>
-      </c>
-      <c r="E99">
-        <v>604.85400000000004</v>
-      </c>
-      <c r="F99">
-        <v>47.061999999999998</v>
-      </c>
-      <c r="G99">
-        <v>508</v>
-      </c>
-      <c r="H99">
-        <v>691</v>
-      </c>
-      <c r="I99">
-        <v>465.54500000000002</v>
-      </c>
+        <v>26.079999999999984</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11">
       <c r="J99">
-        <v>0</v>
-      </c>
-      <c r="K99">
-        <f t="shared" si="2"/>
-        <v>139.30900000000003</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11">
-      <c r="B100">
-        <v>2</v>
-      </c>
-      <c r="C100" t="s">
-        <v>119</v>
-      </c>
-      <c r="D100">
-        <v>173</v>
-      </c>
-      <c r="E100">
-        <v>500.08699999999999</v>
-      </c>
-      <c r="F100">
-        <v>21.128</v>
-      </c>
-      <c r="G100">
-        <v>453</v>
-      </c>
-      <c r="H100">
-        <v>560</v>
-      </c>
-      <c r="I100">
-        <v>461.05399999999997</v>
-      </c>
-      <c r="J100">
-        <v>0</v>
-      </c>
-      <c r="K100">
-        <f t="shared" si="2"/>
-        <v>39.033000000000015</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11">
-      <c r="B101">
-        <v>3</v>
-      </c>
-      <c r="C101" t="s">
-        <v>120</v>
-      </c>
-      <c r="D101">
-        <v>123</v>
-      </c>
-      <c r="E101">
-        <v>485.512</v>
-      </c>
-      <c r="F101">
-        <v>16.664000000000001</v>
-      </c>
-      <c r="G101">
-        <v>441</v>
-      </c>
-      <c r="H101">
-        <v>532</v>
-      </c>
-      <c r="I101">
-        <v>459.43200000000002</v>
-      </c>
-      <c r="J101">
-        <v>0</v>
-      </c>
-      <c r="K101">
-        <f t="shared" si="2"/>
-        <v>26.079999999999984</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11">
-      <c r="J102">
-        <f>SUM(J2:J101)</f>
+        <f>SUM(J2:J98)</f>
         <v>23</v>
       </c>
     </row>

</xml_diff>